<commit_message>
Statistics: Python Tools: Additional Properties
</commit_message>
<xml_diff>
--- a/python/math/trend/50-examples-properties.xlsx
+++ b/python/math/trend/50-examples-properties.xlsx
@@ -13,7 +13,8 @@
     <sheet name="built-in" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="prop" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="alternate" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="compare" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="additional" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="compare" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="231">
   <si>
     <t xml:space="preserve">Least Square</t>
   </si>
@@ -595,6 +596,138 @@
   </si>
   <si>
     <t xml:space="preserve">Mean Squared Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xᵢ freq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yᵢ freq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=MIN(x_sample)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=MIN(y_sample)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=MAX(x_sample)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=MAX(y_sample)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=MAX(x_sample)-MIN(x_sample)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=MAX(y_sample)-MIN(y_sample)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=MEDIAN(x_sample)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=MEDIAN(y_sample)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=MODE(x_sample)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=MODE(y_sample)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x mode (alternative)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=INDEX(x_sample, MATCH(MAX(x_freq), x_freq, 0))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y mode (alternative)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=INDEX(y_sample, MATCH(MAX(y_freq), y_freq, 0))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x SE Mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=STDEV.S(x_sample) / SQRT(COUNT(x_sample))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y SE Mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=STDEV.S(y_sample) / SQRT(COUNT(y_sample))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x kurtosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=KURT(x_sample)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y kurtosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=KURT(y_sample)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x skewness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SKEW(x_sample)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y skewness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SKEW(y_sample)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE kurtosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SQRT((24*(n*(n-2)*(n-3)))/((n+1)*(n+3)*(n-1)^2))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE skewness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SQRT((6*n*(n-1))/((n-2)*(n+1)*(n+3)))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE kurtosis (gaussian)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SQRT(4*(n^2-1)*SE_s^2/((n-3)*(n+5))</t>
   </si>
   <si>
     <t xml:space="preserve">Linear Equation</t>
@@ -1176,7 +1309,7 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF9E9E9E"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF0D47A1"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -1190,7 +1323,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="x_observed" displayName="x_observed" ref="B7:B19" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="x_freq" displayName="x_freq" ref="D7:D22" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name="Column1"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="y_sample_2" displayName="y_sample_2" ref="C7:C22" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>
@@ -1198,7 +1339,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="x_sample" displayName="x_sample" ref="B7:B19" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="x_observed" displayName="x_observed" ref="B7:B19" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>
@@ -1206,7 +1347,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="y_fit" displayName="y_fit" ref="D7:D19" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="x_sample" displayName="x_sample" ref="B7:B19" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>
@@ -1214,7 +1355,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="y_observed" displayName="y_observed" ref="C7:C19" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="x_sample_2" displayName="x_sample_2" ref="B7:B22" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>
@@ -1222,7 +1363,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="y_predicted" displayName="y_predicted" ref="D7:D19" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="y_fit" displayName="y_fit" ref="D7:D19" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>
@@ -1230,7 +1371,31 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="y_sample" displayName="y_sample" ref="C7:C19" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="y_freq" displayName="y_freq" ref="E7:E22" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name="Column1"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="y_observed" displayName="y_observed" ref="C7:C19" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name="Column1"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="y_predicted" displayName="y_predicted" ref="D7:D19" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name="Column1"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="y_sample" displayName="y_sample" ref="C7:C19" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>
@@ -1352,7 +1517,7 @@
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2634,7 +2799,7 @@
       </c>
       <c r="M30" s="21" t="n">
         <f aca="false">M26/(K30*L30)</f>
-        <v>0.970427962120067</v>
+        <v>0.970427962120068</v>
       </c>
       <c r="N30" s="4"/>
       <c r="O30" s="3"/>
@@ -2709,7 +2874,7 @@
       <c r="L33" s="24"/>
       <c r="M33" s="21" t="n">
         <f aca="false">M30^2</f>
-        <v>0.941730429664507</v>
+        <v>0.941730429664508</v>
       </c>
       <c r="N33" s="4"/>
       <c r="O33" s="3"/>
@@ -2768,7 +2933,7 @@
       <c r="L35" s="24"/>
       <c r="M35" s="21" t="n">
         <f aca="false">1-(1-M33)*(B26-1)/(B26-1-1)</f>
-        <v>0.936433195997644</v>
+        <v>0.936433195997646</v>
       </c>
       <c r="N35" s="4"/>
       <c r="O35" s="3"/>
@@ -2956,7 +3121,7 @@
       </c>
       <c r="D7" s="12" t="n">
         <f aca="false">$G$18+$G$17*B7</f>
-        <v>-61</v>
+        <v>-43501</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="34" t="s">
@@ -2982,7 +3147,7 @@
       </c>
       <c r="D8" s="12" t="n">
         <f aca="false">$G$18+$G$17*B8</f>
-        <v>-21</v>
+        <v>-36221</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="34" t="s">
@@ -3008,7 +3173,7 @@
       </c>
       <c r="D9" s="12" t="n">
         <f aca="false">$G$18+$G$17*B9</f>
-        <v>19</v>
+        <v>-28941</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="34" t="s">
@@ -3034,7 +3199,7 @@
       </c>
       <c r="D10" s="12" t="n">
         <f aca="false">$G$18+$G$17*B10</f>
-        <v>59</v>
+        <v>-21661</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="34" t="s">
@@ -3060,7 +3225,7 @@
       </c>
       <c r="D11" s="12" t="n">
         <f aca="false">$G$18+$G$17*B11</f>
-        <v>99</v>
+        <v>-14381</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="34" t="s">
@@ -3086,7 +3251,7 @@
       </c>
       <c r="D12" s="12" t="n">
         <f aca="false">$G$18+$G$17*B12</f>
-        <v>139</v>
+        <v>-7101</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="34" t="s">
@@ -3138,7 +3303,7 @@
       </c>
       <c r="D14" s="12" t="n">
         <f aca="false">$G$18+$G$17*B14</f>
-        <v>219</v>
+        <v>7459</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="34" t="s">
@@ -3146,7 +3311,7 @@
       </c>
       <c r="G14" s="38" t="n">
         <f aca="false">SUMSQ(x_observed-$G$12)</f>
-        <v>182</v>
+        <v>1</v>
       </c>
       <c r="H14" s="39"/>
       <c r="I14" s="40" t="s">
@@ -3164,7 +3329,7 @@
       </c>
       <c r="D15" s="12" t="n">
         <f aca="false">$G$18+$G$17*B15</f>
-        <v>259</v>
+        <v>14739</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="34" t="s">
@@ -3172,7 +3337,7 @@
       </c>
       <c r="G15" s="38" t="n">
         <f aca="false">SUMSQ(y_observed-$G$13)</f>
-        <v>309218</v>
+        <v>2500</v>
       </c>
       <c r="H15" s="39"/>
       <c r="I15" s="40" t="s">
@@ -3190,7 +3355,7 @@
       </c>
       <c r="D16" s="12" t="n">
         <f aca="false">$G$18+$G$17*B16</f>
-        <v>299</v>
+        <v>22019</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="34" t="s">
@@ -3216,7 +3381,7 @@
       </c>
       <c r="D17" s="12" t="n">
         <f aca="false">$G$18+$G$17*B17</f>
-        <v>339</v>
+        <v>29299</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="34" t="s">
@@ -3224,7 +3389,7 @@
       </c>
       <c r="G17" s="38" t="n">
         <f aca="false">G16/G14</f>
-        <v>40</v>
+        <v>7280</v>
       </c>
       <c r="H17" s="39"/>
       <c r="I17" s="40" t="s">
@@ -3242,7 +3407,7 @@
       </c>
       <c r="D18" s="12" t="n">
         <f aca="false">$G$18+$G$17*B18</f>
-        <v>379</v>
+        <v>36579</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="34" t="s">
@@ -3250,7 +3415,7 @@
       </c>
       <c r="G18" s="38" t="n">
         <f aca="false">G13-G17*G12</f>
-        <v>-61</v>
+        <v>-43501</v>
       </c>
       <c r="H18" s="39"/>
       <c r="I18" s="40" t="s">
@@ -3268,7 +3433,7 @@
       </c>
       <c r="D19" s="12" t="n">
         <f aca="false">$G$18+$G$17*B19</f>
-        <v>419</v>
+        <v>43859</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="34" t="s">
@@ -3276,7 +3441,7 @@
       </c>
       <c r="G19" s="38" t="n">
         <f aca="false">G14/G10</f>
-        <v>15.1666666666667</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="H19" s="39"/>
       <c r="I19" s="40" t="s">
@@ -3295,7 +3460,7 @@
       </c>
       <c r="G20" s="38" t="n">
         <f aca="false">G15/G10</f>
-        <v>25768.1666666667</v>
+        <v>208.333333333333</v>
       </c>
       <c r="H20" s="39"/>
       <c r="I20" s="40" t="s">
@@ -3333,7 +3498,7 @@
       </c>
       <c r="G22" s="38" t="n">
         <f aca="false">SQRT(G19)</f>
-        <v>3.89444048184931</v>
+        <v>0.288675134594813</v>
       </c>
       <c r="H22" s="39"/>
       <c r="I22" s="40" t="s">
@@ -3352,7 +3517,7 @@
       </c>
       <c r="G23" s="38" t="n">
         <f aca="false">SQRT(G20)</f>
-        <v>160.524660618444</v>
+        <v>14.4337567297406</v>
       </c>
       <c r="H23" s="39"/>
       <c r="I23" s="40" t="s">
@@ -3371,7 +3536,7 @@
       </c>
       <c r="G24" s="38" t="n">
         <f aca="false">G21/(G22*G23)</f>
-        <v>0.970427962120068</v>
+        <v>145.6</v>
       </c>
       <c r="H24" s="39"/>
       <c r="I24" s="40" t="s">
@@ -3390,7 +3555,7 @@
       </c>
       <c r="G25" s="41" t="n">
         <f aca="false">G24^2</f>
-        <v>0.941730429664508</v>
+        <v>21199.36</v>
       </c>
       <c r="H25" s="39"/>
       <c r="I25" s="40" t="s">
@@ -3409,7 +3574,7 @@
       </c>
       <c r="G26" s="41" t="n">
         <f aca="false">1-(1-G25)*G10/G11</f>
-        <v>0.936433195997646</v>
+        <v>23126.4836363636</v>
       </c>
       <c r="H26" s="39"/>
       <c r="I26" s="40" t="s">
@@ -3426,9 +3591,9 @@
       <c r="F27" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="G27" s="38" t="n">
+      <c r="G27" s="38" t="e">
         <f aca="false">SUMSQ(y_observed-y_predicted)</f>
-        <v>18018</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H27" s="39"/>
       <c r="I27" s="40" t="s">
@@ -3445,9 +3610,9 @@
       <c r="F28" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="G28" s="38" t="n">
+      <c r="G28" s="38" t="e">
         <f aca="false">G27/G11</f>
-        <v>1638</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H28" s="39"/>
       <c r="I28" s="40" t="s">
@@ -3464,9 +3629,9 @@
       <c r="F29" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="G29" s="38" t="n">
+      <c r="G29" s="38" t="e">
         <f aca="false">SQRT(G28/G14)</f>
-        <v>3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H29" s="39"/>
       <c r="I29" s="40" t="s">
@@ -3483,9 +3648,9 @@
       <c r="F30" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="G30" s="38" t="n">
+      <c r="G30" s="38" t="e">
         <f aca="false">G17/G29</f>
-        <v>13.3333333333333</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H30" s="39"/>
       <c r="I30" s="40" t="s">
@@ -3502,9 +3667,9 @@
       <c r="F31" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="G31" s="42" t="n">
+      <c r="G31" s="42" t="e">
         <f aca="false">_xlfn.T.DIST.2T(G30,G11)</f>
-        <v>3.91117071946834E-008</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H31" s="43"/>
       <c r="I31" s="44" t="s">
@@ -3553,7 +3718,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3861,8 +4026,8 @@
         <v>21</v>
       </c>
       <c r="G14" s="38" t="n">
-        <f aca="false" t="array" ref="G14:G14">SUMSQ(x_sample-$G$12)</f>
-        <v>182</v>
+        <f aca="false">SUMSQ(x_sample-$G$12)</f>
+        <v>1</v>
       </c>
       <c r="H14" s="39"/>
       <c r="I14" s="40" t="s">
@@ -3887,8 +4052,8 @@
         <v>23</v>
       </c>
       <c r="G15" s="38" t="n">
-        <f aca="false" t="array" ref="G15:G15">SUMSQ(y_sample-$G$13)</f>
-        <v>309218</v>
+        <f aca="false">SUMSQ(y_sample-$G$13)</f>
+        <v>2500</v>
       </c>
       <c r="H15" s="39"/>
       <c r="I15" s="40" t="s">
@@ -4142,9 +4307,9 @@
       <c r="F27" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="G27" s="38" t="n">
-        <f aca="false" t="array" ref="G27:G27">SUMSQ(y_sample-y_fit)</f>
-        <v>18018</v>
+      <c r="G27" s="38" t="e">
+        <f aca="false">SUMSQ(y_sample-y_fit)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="H27" s="39"/>
       <c r="I27" s="40" t="s">
@@ -4161,9 +4326,9 @@
       <c r="F28" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="G28" s="38" t="n">
+      <c r="G28" s="38" t="e">
         <f aca="false">G27/G11</f>
-        <v>1638</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H28" s="39"/>
       <c r="I28" s="40" t="s">
@@ -4180,9 +4345,9 @@
       <c r="F29" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="G29" s="38" t="n">
+      <c r="G29" s="38" t="e">
         <f aca="false">SQRT(G28/G14)</f>
-        <v>3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H29" s="39"/>
       <c r="I29" s="40" t="s">
@@ -4199,9 +4364,9 @@
       <c r="F30" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="G30" s="38" t="n">
+      <c r="G30" s="38" t="e">
         <f aca="false">G17/G29</f>
-        <v>13.3333333333333</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H30" s="39"/>
       <c r="I30" s="40" t="s">
@@ -4218,9 +4383,9 @@
       <c r="F31" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="G31" s="42" t="n">
+      <c r="G31" s="42" t="e">
         <f aca="false">_xlfn.T.DIST.2T(G30,G11)</f>
-        <v>3.91117071946834E-008</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H31" s="43"/>
       <c r="I31" s="44" t="s">
@@ -4269,7 +4434,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5977,6 +6142,735 @@
     <tabColor rgb="FF1976D2"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:K29"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="2.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="27" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="12.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="45.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="2.56"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="8.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3"/>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="8.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3"/>
+      <c r="B6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="19"/>
+      <c r="J6" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12" t="n">
+        <f aca="false">COUNTIF(x_sample_2,B7)</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <f aca="false">COUNTIF(y_sample_2,C7)</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="H7" s="35" t="n">
+        <f aca="false">MIN(x_sample_2)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="36"/>
+      <c r="J7" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3"/>
+      <c r="B8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="D8" s="12" t="n">
+        <f aca="false">COUNTIF(x_sample_2,B8)</f>
+        <v>1</v>
+      </c>
+      <c r="E8" s="12" t="n">
+        <f aca="false">COUNTIF(y_sample_2,C8)</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="H8" s="35" t="n">
+        <f aca="false">MIN(y_sample_2)</f>
+        <v>5</v>
+      </c>
+      <c r="I8" s="36"/>
+      <c r="J8" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3"/>
+      <c r="B9" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="12" t="n">
+        <v>25</v>
+      </c>
+      <c r="D9" s="12" t="n">
+        <f aca="false">COUNTIF(x_sample_2,B9)</f>
+        <v>1</v>
+      </c>
+      <c r="E9" s="12" t="n">
+        <f aca="false">COUNTIF(y_sample_2,C9)</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="H9" s="35" t="n">
+        <f aca="false">MAX(x_sample_2)</f>
+        <v>12</v>
+      </c>
+      <c r="I9" s="36"/>
+      <c r="J9" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3"/>
+      <c r="B10" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="12" t="n">
+        <v>44</v>
+      </c>
+      <c r="D10" s="12" t="n">
+        <f aca="false">COUNTIF(x_sample_2,B10)</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="12" t="n">
+        <f aca="false">COUNTIF(y_sample_2,C10)</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="H10" s="35" t="n">
+        <f aca="false">MAX(y_sample_2)</f>
+        <v>485</v>
+      </c>
+      <c r="I10" s="36"/>
+      <c r="J10" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3"/>
+      <c r="B11" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="12" t="n">
+        <v>69</v>
+      </c>
+      <c r="D11" s="12" t="n">
+        <f aca="false">COUNTIF(x_sample_2,B11)</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="12" t="n">
+        <f aca="false">COUNTIF(y_sample_2,C11)</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="H11" s="35" t="n">
+        <f aca="false">MAX(x_sample_2)-MIN(x_sample_2)</f>
+        <v>12</v>
+      </c>
+      <c r="I11" s="36"/>
+      <c r="J11" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3"/>
+      <c r="B12" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="D12" s="12" t="n">
+        <f aca="false">COUNTIF(x_sample_2,B12)</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="12" t="n">
+        <f aca="false">COUNTIF(y_sample_2,C12)</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="H12" s="35" t="n">
+        <f aca="false">MAX(y_sample_2)-MIN(y_sample_2)</f>
+        <v>480</v>
+      </c>
+      <c r="I12" s="39"/>
+      <c r="J12" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3"/>
+      <c r="B13" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="C13" s="12" t="n">
+        <v>137</v>
+      </c>
+      <c r="D13" s="12" t="n">
+        <f aca="false">COUNTIF(x_sample_2,B13)</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="12" t="n">
+        <f aca="false">COUNTIF(y_sample_2,C13)</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="H13" s="35" t="n">
+        <f aca="false">MEDIAN(x_sample_2)</f>
+        <v>6</v>
+      </c>
+      <c r="I13" s="36"/>
+      <c r="J13" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3"/>
+      <c r="B14" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="C14" s="12" t="n">
+        <v>180</v>
+      </c>
+      <c r="D14" s="12" t="n">
+        <f aca="false">COUNTIF(x_sample_2,B14)</f>
+        <v>1</v>
+      </c>
+      <c r="E14" s="12" t="n">
+        <f aca="false">COUNTIF(y_sample_2,C14)</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="H14" s="35" t="n">
+        <f aca="false">MEDIAN(y_sample_2)</f>
+        <v>137</v>
+      </c>
+      <c r="I14" s="36"/>
+      <c r="J14" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3"/>
+      <c r="B15" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="C15" s="12" t="n">
+        <v>229</v>
+      </c>
+      <c r="D15" s="12" t="n">
+        <f aca="false">COUNTIF(x_sample_2,B15)</f>
+        <v>1</v>
+      </c>
+      <c r="E15" s="12" t="n">
+        <f aca="false">COUNTIF(y_sample_2,C15)</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="H15" s="35" t="e">
+        <f aca="false">MODE(B7:B19)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I15" s="39"/>
+      <c r="J15" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3"/>
+      <c r="B16" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C16" s="12" t="n">
+        <v>284</v>
+      </c>
+      <c r="D16" s="12" t="n">
+        <f aca="false">COUNTIF(x_sample_2,B16)</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="12" t="n">
+        <f aca="false">COUNTIF(y_sample_2,C16)</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="H16" s="35" t="e">
+        <f aca="false">MODE(C7:C19)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I16" s="39"/>
+      <c r="J16" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3"/>
+      <c r="B17" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C17" s="12" t="n">
+        <v>345</v>
+      </c>
+      <c r="D17" s="12" t="n">
+        <f aca="false">COUNTIF(x_sample_2,B17)</f>
+        <v>1</v>
+      </c>
+      <c r="E17" s="12" t="n">
+        <f aca="false">COUNTIF(y_sample_2,C17)</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="H17" s="35" t="n">
+        <f aca="false">INDEX(x_sample_2, MATCH(MAX(x_freq), x_freq, 0))</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="39"/>
+      <c r="J17" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3"/>
+      <c r="B18" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="C18" s="12" t="n">
+        <v>412</v>
+      </c>
+      <c r="D18" s="12" t="n">
+        <f aca="false">COUNTIF(x_sample_2,B18)</f>
+        <v>1</v>
+      </c>
+      <c r="E18" s="12" t="n">
+        <f aca="false">COUNTIF(y_sample_2,C18)</f>
+        <v>1</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="H18" s="35" t="n">
+        <f aca="false">INDEX(y_sample_2, MATCH(MAX(y_freq), y_freq, 0))</f>
+        <v>5</v>
+      </c>
+      <c r="I18" s="39"/>
+      <c r="J18" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3"/>
+      <c r="B19" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="C19" s="12" t="n">
+        <v>485</v>
+      </c>
+      <c r="D19" s="12" t="n">
+        <f aca="false">COUNTIF(x_sample_2,B19)</f>
+        <v>1</v>
+      </c>
+      <c r="E19" s="12" t="n">
+        <f aca="false">COUNTIF(y_sample_2,C19)</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="H19" s="38" t="n">
+        <f aca="false">_xlfn.STDEV.S(x_sample_2) / SQRT(COUNT(x_sample_2))</f>
+        <v>1.08012344973464</v>
+      </c>
+      <c r="I19" s="39"/>
+      <c r="J19" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="34" t="s">
+        <v>194</v>
+      </c>
+      <c r="H20" s="38" t="n">
+        <f aca="false">_xlfn.STDEV.S(y_sample_2) / SQRT(COUNT(y_sample_2))</f>
+        <v>44.5215303720196</v>
+      </c>
+      <c r="I20" s="39"/>
+      <c r="J20" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="H21" s="38" t="n">
+        <f aca="false">KURT(x_sample_2)</f>
+        <v>-1.2</v>
+      </c>
+      <c r="I21" s="39"/>
+      <c r="J21" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="H22" s="38" t="n">
+        <f aca="false">KURT(y_sample_2)</f>
+        <v>-0.733703044811924</v>
+      </c>
+      <c r="I22" s="39"/>
+      <c r="J22" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="H23" s="38" t="n">
+        <f aca="false">SKEW(x_sample_2)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="39"/>
+      <c r="J23" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="H24" s="38" t="n">
+        <f aca="false">SKEW(y_sample_2)</f>
+        <v>0.695766189129513</v>
+      </c>
+      <c r="I24" s="39"/>
+      <c r="J24" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="38" t="n">
+        <f aca="false">COUNT(x_sample_2)</f>
+        <v>13</v>
+      </c>
+      <c r="I25" s="39"/>
+      <c r="J25" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="H26" s="38" t="n">
+        <f aca="false">SQRT((24*(H25*(H25-2)*(H25-3)))/((H25+1)*(H25+3)*(H25-1)^2))</f>
+        <v>1.03149798605625</v>
+      </c>
+      <c r="I26" s="39"/>
+      <c r="J26" s="40" t="s">
+        <v>205</v>
+      </c>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="H27" s="38" t="n">
+        <f aca="false">SQRT((6*H25*(H25-1))/((H25-2)*(H25+1)*(H25+3)))</f>
+        <v>0.616336052709989</v>
+      </c>
+      <c r="I27" s="39"/>
+      <c r="J27" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="H28" s="38" t="n">
+        <f aca="false">SQRT(4*(H25^2-1)*H27^2/((H25-3)*(H25+5)))</f>
+        <v>1.1908743922773</v>
+      </c>
+      <c r="I28" s="39"/>
+      <c r="J28" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" customFormat="false" ht="8.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="G5:J5"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FF0D47A1"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -6033,20 +6927,20 @@
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="45"/>
       <c r="B4" s="59" t="s">
-        <v>166</v>
+        <v>210</v>
       </c>
       <c r="C4" s="60"/>
       <c r="E4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="59" t="s">
-        <v>167</v>
+        <v>211</v>
       </c>
       <c r="K4" s="61"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="59" t="s">
-        <v>168</v>
+        <v>212</v>
       </c>
       <c r="S4" s="61"/>
       <c r="T4" s="2"/>
@@ -6056,17 +6950,17 @@
     <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="45"/>
       <c r="B5" s="4" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="E5" s="2"/>
       <c r="I5" s="45"/>
       <c r="J5" s="4" t="s">
-        <v>170</v>
+        <v>214</v>
       </c>
       <c r="M5" s="2"/>
       <c r="Q5" s="45"/>
       <c r="R5" s="4" t="s">
-        <v>171</v>
+        <v>215</v>
       </c>
       <c r="U5" s="2"/>
       <c r="Y5" s="2"/>
@@ -6083,7 +6977,7 @@
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="45"/>
       <c r="B7" s="7" t="s">
-        <v>172</v>
+        <v>216</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>69</v>
@@ -6091,7 +6985,7 @@
       <c r="E7" s="2"/>
       <c r="I7" s="45"/>
       <c r="J7" s="7" t="s">
-        <v>172</v>
+        <v>216</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>69</v>
@@ -6099,7 +6993,7 @@
       <c r="M7" s="2"/>
       <c r="Q7" s="45"/>
       <c r="R7" s="7" t="s">
-        <v>172</v>
+        <v>216</v>
       </c>
       <c r="S7" s="8" t="s">
         <v>69</v>
@@ -6110,7 +7004,7 @@
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="45"/>
       <c r="B8" s="62" t="s">
-        <v>173</v>
+        <v>217</v>
       </c>
       <c r="C8" s="12" t="n">
         <v>5</v>
@@ -6118,7 +7012,7 @@
       <c r="E8" s="2"/>
       <c r="I8" s="45"/>
       <c r="J8" s="62" t="s">
-        <v>173</v>
+        <v>217</v>
       </c>
       <c r="K8" s="12" t="n">
         <v>5</v>
@@ -6126,7 +7020,7 @@
       <c r="M8" s="2"/>
       <c r="Q8" s="45"/>
       <c r="R8" s="62" t="s">
-        <v>173</v>
+        <v>217</v>
       </c>
       <c r="S8" s="12" t="n">
         <v>5</v>
@@ -6168,7 +7062,7 @@
       <c r="E10" s="2"/>
       <c r="I10" s="45"/>
       <c r="J10" s="62" t="s">
-        <v>174</v>
+        <v>218</v>
       </c>
       <c r="K10" s="12" t="n">
         <v>3</v>
@@ -6176,7 +7070,7 @@
       <c r="M10" s="2"/>
       <c r="Q10" s="45"/>
       <c r="R10" s="62" t="s">
-        <v>174</v>
+        <v>218</v>
       </c>
       <c r="S10" s="12" t="n">
         <v>3</v>
@@ -6195,7 +7089,7 @@
       <c r="M11" s="2"/>
       <c r="Q11" s="45"/>
       <c r="R11" s="62" t="s">
-        <v>175</v>
+        <v>219</v>
       </c>
       <c r="S11" s="12" t="n">
         <v>2</v>
@@ -6277,7 +7171,7 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="34" t="s">
-        <v>176</v>
+        <v>220</v>
       </c>
       <c r="G14" s="21" t="n">
         <f aca="false">SUM(B14:B26)</f>
@@ -6294,7 +7188,7 @@
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="34" t="s">
-        <v>176</v>
+        <v>220</v>
       </c>
       <c r="O14" s="21" t="n">
         <f aca="false">SUM(J14:J26)</f>
@@ -6311,7 +7205,7 @@
       </c>
       <c r="U14" s="2"/>
       <c r="V14" s="34" t="s">
-        <v>176</v>
+        <v>220</v>
       </c>
       <c r="W14" s="21" t="n">
         <f aca="false">SUM(R14:R26)</f>
@@ -6332,7 +7226,7 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="34" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
       <c r="G15" s="21" t="n">
         <f aca="false">SUM(C14:C26)</f>
@@ -6350,7 +7244,7 @@
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="34" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
       <c r="O15" s="21" t="n">
         <f aca="false">SUM(K14:K26)</f>
@@ -6368,7 +7262,7 @@
       </c>
       <c r="U15" s="2"/>
       <c r="V15" s="34" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
       <c r="W15" s="21" t="n">
         <f aca="false">SUM(S14:S26)</f>
@@ -6389,7 +7283,7 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="34" t="s">
-        <v>178</v>
+        <v>222</v>
       </c>
       <c r="G16" s="21" t="n">
         <f aca="false">COUNT(B14:B26)</f>
@@ -6407,7 +7301,7 @@
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="34" t="s">
-        <v>178</v>
+        <v>222</v>
       </c>
       <c r="O16" s="21" t="n">
         <f aca="false">COUNT(J14:J26)</f>
@@ -6425,7 +7319,7 @@
       </c>
       <c r="U16" s="2"/>
       <c r="V16" s="34" t="s">
-        <v>178</v>
+        <v>222</v>
       </c>
       <c r="W16" s="21" t="n">
         <f aca="false">COUNT(R14:R26)</f>
@@ -6446,7 +7340,7 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="34" t="s">
-        <v>179</v>
+        <v>223</v>
       </c>
       <c r="G17" s="21" t="n">
         <f aca="false">COUNT(C14:C26)</f>
@@ -6464,7 +7358,7 @@
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="34" t="s">
-        <v>179</v>
+        <v>223</v>
       </c>
       <c r="O17" s="21" t="n">
         <f aca="false">COUNT(K14:K26)</f>
@@ -6482,7 +7376,7 @@
       </c>
       <c r="U17" s="2"/>
       <c r="V17" s="34" t="s">
-        <v>179</v>
+        <v>223</v>
       </c>
       <c r="W17" s="21" t="n">
         <f aca="false">COUNT(S14:S26)</f>
@@ -6503,7 +7397,7 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="34" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="G18" s="21" t="n">
         <f aca="false">AVERAGE(B14:B26)</f>
@@ -6524,7 +7418,7 @@
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="34" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="O18" s="21" t="n">
         <f aca="false">AVERAGE(J14:J26)</f>
@@ -6545,7 +7439,7 @@
       </c>
       <c r="U18" s="2"/>
       <c r="V18" s="34" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="W18" s="21" t="n">
         <f aca="false">AVERAGE(R14:R26)</f>
@@ -6569,7 +7463,7 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="34" t="s">
-        <v>181</v>
+        <v>225</v>
       </c>
       <c r="G19" s="21" t="n">
         <f aca="false">AVERAGE(C14:C26)</f>
@@ -6590,7 +7484,7 @@
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="34" t="s">
-        <v>181</v>
+        <v>225</v>
       </c>
       <c r="O19" s="21" t="n">
         <f aca="false">AVERAGE(K14:K26)</f>
@@ -6611,7 +7505,7 @@
       </c>
       <c r="U19" s="2"/>
       <c r="V19" s="34" t="s">
-        <v>181</v>
+        <v>225</v>
       </c>
       <c r="W19" s="21" t="n">
         <f aca="false">AVERAGE(S14:S26)</f>
@@ -6635,7 +7529,7 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="34" t="s">
-        <v>182</v>
+        <v>226</v>
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">_xlfn.VAR.S(B14:B26)</f>
@@ -6656,7 +7550,7 @@
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="34" t="s">
-        <v>182</v>
+        <v>226</v>
       </c>
       <c r="O20" s="21" t="n">
         <f aca="false">_xlfn.VAR.S(J14:J26)</f>
@@ -6677,7 +7571,7 @@
       </c>
       <c r="U20" s="2"/>
       <c r="V20" s="34" t="s">
-        <v>182</v>
+        <v>226</v>
       </c>
       <c r="W20" s="21" t="n">
         <f aca="false">_xlfn.VAR.S(R14:R26)</f>
@@ -6701,7 +7595,7 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="34" t="s">
-        <v>183</v>
+        <v>227</v>
       </c>
       <c r="G21" s="21" t="n">
         <f aca="false">_xlfn.VAR.S(C14:C26)</f>
@@ -6722,7 +7616,7 @@
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="34" t="s">
-        <v>183</v>
+        <v>227</v>
       </c>
       <c r="O21" s="21" t="n">
         <f aca="false">_xlfn.VAR.S(K14:K26)</f>
@@ -6743,7 +7637,7 @@
       </c>
       <c r="U21" s="2"/>
       <c r="V21" s="34" t="s">
-        <v>183</v>
+        <v>227</v>
       </c>
       <c r="W21" s="21" t="n">
         <f aca="false">_xlfn.VAR.S(S14:S26)</f>
@@ -6767,7 +7661,7 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="34" t="s">
-        <v>184</v>
+        <v>228</v>
       </c>
       <c r="G22" s="21" t="n">
         <f aca="false">_xlfn.STDEV.S(B14:B26)</f>
@@ -6788,7 +7682,7 @@
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="34" t="s">
-        <v>184</v>
+        <v>228</v>
       </c>
       <c r="O22" s="21" t="n">
         <f aca="false">_xlfn.STDEV.S(J14:J26)</f>
@@ -6809,7 +7703,7 @@
       </c>
       <c r="U22" s="2"/>
       <c r="V22" s="34" t="s">
-        <v>184</v>
+        <v>228</v>
       </c>
       <c r="W22" s="21" t="n">
         <f aca="false">_xlfn.STDEV.S(R14:R26)</f>
@@ -6833,7 +7727,7 @@
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="34" t="s">
-        <v>185</v>
+        <v>229</v>
       </c>
       <c r="G23" s="21" t="n">
         <f aca="false">_xlfn.STDEV.S(C14:C26)</f>
@@ -6854,7 +7748,7 @@
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="34" t="s">
-        <v>185</v>
+        <v>229</v>
       </c>
       <c r="O23" s="21" t="n">
         <f aca="false">_xlfn.STDEV.S(K14:K26)</f>
@@ -6875,7 +7769,7 @@
       </c>
       <c r="U23" s="2"/>
       <c r="V23" s="34" t="s">
-        <v>185</v>
+        <v>229</v>
       </c>
       <c r="W23" s="21" t="n">
         <f aca="false">_xlfn.STDEV.S(S14:S26)</f>
@@ -7076,7 +7970,7 @@
       <c r="C27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="34" t="s">
-        <v>186</v>
+        <v>230</v>
       </c>
       <c r="G27" s="21" t="n">
         <f aca="false">SLOPE(B14:B26,C14:C26)</f>
@@ -7091,7 +7985,7 @@
       <c r="K27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="34" t="s">
-        <v>186</v>
+        <v>230</v>
       </c>
       <c r="O27" s="21" t="n">
         <f aca="false">SLOPE(J14:J26,K14:K26)</f>
@@ -7106,7 +8000,7 @@
       <c r="S27" s="2"/>
       <c r="U27" s="2"/>
       <c r="V27" s="34" t="s">
-        <v>186</v>
+        <v>230</v>
       </c>
       <c r="W27" s="21" t="n">
         <f aca="false">SLOPE(R14:R26,S14:S26)</f>

</xml_diff>